<commit_message>
NAD_letterID_v1 reliability testing updated
</commit_message>
<xml_diff>
--- a/reliability_testing/task_indices_psychometric_analysis_results.xlsx
+++ b/reliability_testing/task_indices_psychometric_analysis_results.xlsx
@@ -713,7 +713,7 @@
         <v>35</v>
       </c>
       <c r="E8" s="2">
-        <v>0.68968296532168805</v>
+        <v>0.69861010172082794</v>
       </c>
       <c r="F8">
         <f t="shared" ref="F8:F71" si="1">IF(E8="","n.a.",IF(E8&lt;0.7,0,1))</f>
@@ -734,7 +734,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="2">
-        <v>0.79394920822215154</v>
+        <v>0.79771876635528216</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
@@ -755,7 +755,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="2">
-        <v>0.77482339944313938</v>
+        <v>0.77324957432738162</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
@@ -776,7 +776,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="2">
-        <v>0.82687727403715194</v>
+        <v>0.82523623856074635</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
@@ -797,7 +797,7 @@
         <v>35</v>
       </c>
       <c r="E12" s="2">
-        <v>0.77521333153418281</v>
+        <v>0.77418707741092208</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
@@ -818,7 +818,7 @@
         <v>35</v>
       </c>
       <c r="E13" s="2">
-        <v>0.77715421241518079</v>
+        <v>0.77517705116729763</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
@@ -951,7 +951,7 @@
         <v>35</v>
       </c>
       <c r="E21" s="2">
-        <v>0.62855292840611876</v>
+        <v>0.615162923666559</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
@@ -972,7 +972,7 @@
         <v>35</v>
       </c>
       <c r="E22" s="2">
-        <v>0.63777081364340005</v>
+        <v>0.6407323614837136</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
@@ -993,7 +993,7 @@
         <v>35</v>
       </c>
       <c r="E23" s="2">
-        <v>0.71050110990299897</v>
+        <v>0.70506102686013872</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
@@ -1014,7 +1014,7 @@
         <v>35</v>
       </c>
       <c r="E24" s="2">
-        <v>0.85457112827674131</v>
+        <v>0.85260893707265906</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
@@ -1035,7 +1035,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="2">
-        <v>0.77727138967244924</v>
+        <v>0.77024989616050177</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
@@ -1056,7 +1056,7 @@
         <v>35</v>
       </c>
       <c r="E26" s="2">
-        <v>0.73030107410643075</v>
+        <v>0.72315531293363244</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
@@ -1189,7 +1189,7 @@
         <v>35</v>
       </c>
       <c r="E34" s="2">
-        <v>0.88377151915230445</v>
+        <v>0.88541539422498994</v>
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
@@ -1210,7 +1210,7 @@
         <v>35</v>
       </c>
       <c r="E35" s="2">
-        <v>0.93138816423470216</v>
+        <v>0.93006256688195676</v>
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
@@ -1231,7 +1231,7 @@
         <v>35</v>
       </c>
       <c r="E36" s="2">
-        <v>0.90333788895638645</v>
+        <v>0.90150188613479521</v>
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
@@ -1252,7 +1252,7 @@
         <v>35</v>
       </c>
       <c r="E37" s="2">
-        <v>0.65745332040991855</v>
+        <v>0.6565218803097731</v>
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
@@ -1273,7 +1273,7 @@
         <v>35</v>
       </c>
       <c r="E38" s="2">
-        <v>0.6410009318145623</v>
+        <v>0.64430526037663449</v>
       </c>
       <c r="F38">
         <f t="shared" si="1"/>
@@ -1294,7 +1294,7 @@
         <v>35</v>
       </c>
       <c r="E39" s="2">
-        <v>0.70600146265921526</v>
+        <v>0.70786188269463246</v>
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
@@ -1427,7 +1427,7 @@
         <v>35</v>
       </c>
       <c r="E47" s="2">
-        <v>0.38163998557494</v>
+        <v>0.37984454924567129</v>
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
@@ -1448,7 +1448,7 @@
         <v>35</v>
       </c>
       <c r="E48" s="2">
-        <v>0.47021387639616358</v>
+        <v>0.46614680711297962</v>
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
@@ -1469,7 +1469,7 @@
         <v>35</v>
       </c>
       <c r="E49" s="2">
-        <v>0.38590122441754188</v>
+        <v>0.384960776705147</v>
       </c>
       <c r="F49">
         <f t="shared" si="1"/>
@@ -1490,7 +1490,7 @@
         <v>35</v>
       </c>
       <c r="E50" s="2">
-        <v>0.66693040978983731</v>
+        <v>0.67022087260984964</v>
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
@@ -1511,7 +1511,7 @@
         <v>35</v>
       </c>
       <c r="E51" s="2">
-        <v>0.4843387370556379</v>
+        <v>0.48956448606352948</v>
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
@@ -1532,7 +1532,7 @@
         <v>35</v>
       </c>
       <c r="E52" s="2">
-        <v>0.50032292418690938</v>
+        <v>0.48947414177980991</v>
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
@@ -1601,7 +1601,7 @@
         <v>35</v>
       </c>
       <c r="E56" s="2">
-        <v>0.69439297114564247</v>
+        <v>0.67974292441480011</v>
       </c>
       <c r="F56">
         <f t="shared" si="1"/>
@@ -1622,7 +1622,7 @@
         <v>35</v>
       </c>
       <c r="E57" s="2">
-        <v>0.73811715773359154</v>
+        <v>0.73723652377610138</v>
       </c>
       <c r="F57">
         <f t="shared" si="1"/>
@@ -1643,11 +1643,11 @@
         <v>35</v>
       </c>
       <c r="E58" s="2">
-        <v>0.70917552915408955</v>
+        <v>0.6895504117134762</v>
       </c>
       <c r="F58">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1664,7 +1664,7 @@
         <v>35</v>
       </c>
       <c r="E59" s="2">
-        <v>0.75889511614818339</v>
+        <v>0.74417042790677312</v>
       </c>
       <c r="F59">
         <f t="shared" si="1"/>
@@ -1685,7 +1685,7 @@
         <v>35</v>
       </c>
       <c r="E60" s="2">
-        <v>0.65720259675006976</v>
+        <v>0.67926217348995077</v>
       </c>
       <c r="F60">
         <f t="shared" si="1"/>
@@ -1706,7 +1706,7 @@
         <v>35</v>
       </c>
       <c r="E61" s="2">
-        <v>0.62462961600986622</v>
+        <v>0.6171899492989581</v>
       </c>
       <c r="F61">
         <f t="shared" si="1"/>

</xml_diff>